<commit_message>
updated db and form_database
</commit_message>
<xml_diff>
--- a/db_files/entries_2022.xlsx
+++ b/db_files/entries_2022.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="entries" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="137">
   <si>
     <t>Czech Republic</t>
   </si>
@@ -67,6 +67,369 @@
   </si>
   <si>
     <t>Way Down</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Albania</t>
+  </si>
+  <si>
+    <t>Ronela Hajati</t>
+  </si>
+  <si>
+    <t>Sekret</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bulgaria</t>
+  </si>
+  <si>
+    <t>Intelligent Music Project</t>
+  </si>
+  <si>
+    <t>Intention</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Latvia</t>
+  </si>
+  <si>
+    <t>Eat Your Salad</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lithuania</t>
+  </si>
+  <si>
+    <t>Monika Liu</t>
+  </si>
+  <si>
+    <t>Sentimentai</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Moldova</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Netherlands</t>
+  </si>
+  <si>
+    <t>S10</t>
+  </si>
+  <si>
+    <t>De diepte</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Slovenia</t>
+  </si>
+  <si>
+    <t>LPS</t>
+  </si>
+  <si>
+    <t>Disko</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Switzerland</t>
+  </si>
+  <si>
+    <t>Marius Bear</t>
+  </si>
+  <si>
+    <t>Boys Do Cry</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ukraine</t>
+  </si>
+  <si>
+    <t>Kalush Orchestra</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Armenia</t>
+  </si>
+  <si>
+    <t>Rosa Linn</t>
+  </si>
+  <si>
+    <t>Snap</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Austria</t>
+  </si>
+  <si>
+    <t>Lumix feat. Pia Maria</t>
+  </si>
+  <si>
+    <t>Halo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Croatia</t>
+  </si>
+  <si>
+    <t>Guilty Pleasure</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Denmark</t>
+  </si>
+  <si>
+    <t>Reddi</t>
+  </si>
+  <si>
+    <t>The Show</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Greece</t>
+  </si>
+  <si>
+    <t>Amanda Georgiadi Tenfjord</t>
+  </si>
+  <si>
+    <t>Die Together</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Iceland</t>
+  </si>
+  <si>
+    <t>Systur</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Norway</t>
+  </si>
+  <si>
+    <t>Subwoolfer</t>
+  </si>
+  <si>
+    <t>Give That Wolf a Banana</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Portugal</t>
+  </si>
+  <si>
+    <t>Maro</t>
+  </si>
+  <si>
+    <t>Saudade, saudade</t>
+  </si>
+  <si>
+    <t>Citi Zēni</t>
+  </si>
+  <si>
+    <t>Zdob și Zdub and Frații Advahov</t>
+  </si>
+  <si>
+    <t>Trenulețul</t>
+  </si>
+  <si>
+    <t>Stefania (Стефанія)</t>
+  </si>
+  <si>
+    <t>Mia Dimšić</t>
+  </si>
+  <si>
+    <t>Með hækkandi sól</t>
+  </si>
+  <si>
+    <t>First Semi-Final</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Australia</t>
+  </si>
+  <si>
+    <t>Sheldon Riley</t>
+  </si>
+  <si>
+    <t>Not the Same</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Azerbaijan</t>
+  </si>
+  <si>
+    <t>Nadir Rustamli</t>
+  </si>
+  <si>
+    <t>Fade to Black</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cyprus</t>
+  </si>
+  <si>
+    <t>Andromache</t>
+  </si>
+  <si>
+    <t>Ela (Έλα)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Finland</t>
+  </si>
+  <si>
+    <t>The Rasmus</t>
+  </si>
+  <si>
+    <t>Jezebel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Georgia</t>
+  </si>
+  <si>
+    <t>Circus Mircus</t>
+  </si>
+  <si>
+    <t>Lock Me In</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Israel</t>
+  </si>
+  <si>
+    <t>Michael Ben David</t>
+  </si>
+  <si>
+    <t>I.M</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Malta</t>
+  </si>
+  <si>
+    <t>Emma Muscat</t>
+  </si>
+  <si>
+    <t>I Am What I Am</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> San Marino</t>
+  </si>
+  <si>
+    <t>Achille Lauro</t>
+  </si>
+  <si>
+    <t>Stripper</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Serbia</t>
+  </si>
+  <si>
+    <t>Konstrakta</t>
+  </si>
+  <si>
+    <t>In corpore sano</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Belgium</t>
+  </si>
+  <si>
+    <t>Jérémie Makiese</t>
+  </si>
+  <si>
+    <t>Miss You</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Czech Republic</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Estonia</t>
+  </si>
+  <si>
+    <t>Stefan</t>
+  </si>
+  <si>
+    <t>Hope</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ireland</t>
+  </si>
+  <si>
+    <t>Brooke</t>
+  </si>
+  <si>
+    <t>That's Rich</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Montenegro</t>
+  </si>
+  <si>
+    <t>Vladana</t>
+  </si>
+  <si>
+    <t>Breathe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> North Macedonia</t>
+  </si>
+  <si>
+    <t>Andrea</t>
+  </si>
+  <si>
+    <t>Circles</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Poland</t>
+  </si>
+  <si>
+    <t>Ochman</t>
+  </si>
+  <si>
+    <t>River</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Romania</t>
+  </si>
+  <si>
+    <t>WRS</t>
+  </si>
+  <si>
+    <t>Llámame</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sweden</t>
+  </si>
+  <si>
+    <t>Cornelia Jakobs</t>
+  </si>
+  <si>
+    <t>Hold Me Closer</t>
+  </si>
+  <si>
+    <t>Second Semi-Final</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Italy</t>
+  </si>
+  <si>
+    <t>Mahmood and Blanco</t>
+  </si>
+  <si>
+    <t>Brividi</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> France</t>
+  </si>
+  <si>
+    <t>Alvan and Ahez</t>
+  </si>
+  <si>
+    <t>Fulenn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Germany</t>
+  </si>
+  <si>
+    <t>Malik Harris</t>
+  </si>
+  <si>
+    <t>Rockstars</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Spain</t>
+  </si>
+  <si>
+    <t>Chanel</t>
+  </si>
+  <si>
+    <t>SloMo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> United Kingdom</t>
+  </si>
+  <si>
+    <t>Sam Ryder</t>
+  </si>
+  <si>
+    <t>Space Man</t>
+  </si>
+  <si>
+    <t>Grand Final</t>
   </si>
 </sst>
 </file>
@@ -874,19 +1237,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G1:G7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
     <col min="6" max="6" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" bestFit="1" customWidth="1"/>
   </cols>
@@ -1052,6 +1415,926 @@
         <v>0</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8">
+        <v>2022</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9">
+        <v>2022</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10">
+        <v>2022</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11">
+        <v>2022</v>
+      </c>
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12">
+        <v>2022</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13">
+        <v>2022</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14">
+        <v>2022</v>
+      </c>
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15">
+        <v>2022</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16">
+        <v>2022</v>
+      </c>
+      <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17">
+        <v>2022</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18">
+        <v>2022</v>
+      </c>
+      <c r="C18">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19">
+        <v>2022</v>
+      </c>
+      <c r="C19">
+        <v>12</v>
+      </c>
+      <c r="D19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" t="s">
+        <v>65</v>
+      </c>
+      <c r="F19" t="s">
+        <v>46</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20">
+        <v>2022</v>
+      </c>
+      <c r="C20">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21">
+        <v>2022</v>
+      </c>
+      <c r="C21">
+        <v>14</v>
+      </c>
+      <c r="D21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22">
+        <v>2022</v>
+      </c>
+      <c r="C22">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23">
+        <v>2022</v>
+      </c>
+      <c r="C23">
+        <v>16</v>
+      </c>
+      <c r="D23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" t="s">
+        <v>56</v>
+      </c>
+      <c r="F23" t="s">
+        <v>57</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24">
+        <v>2022</v>
+      </c>
+      <c r="C24">
+        <v>17</v>
+      </c>
+      <c r="D24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25">
+        <v>2022</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" t="s">
+        <v>69</v>
+      </c>
+      <c r="F25" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>120</v>
+      </c>
+      <c r="B26">
+        <v>2022</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>71</v>
+      </c>
+      <c r="E26" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27">
+        <v>2022</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>74</v>
+      </c>
+      <c r="E27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F27" t="s">
+        <v>76</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B28">
+        <v>2022</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" t="s">
+        <v>78</v>
+      </c>
+      <c r="F28" t="s">
+        <v>79</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>120</v>
+      </c>
+      <c r="B29">
+        <v>2022</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" t="s">
+        <v>82</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30">
+        <v>2022</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" t="s">
+        <v>84</v>
+      </c>
+      <c r="F30" t="s">
+        <v>85</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>120</v>
+      </c>
+      <c r="B31">
+        <v>2022</v>
+      </c>
+      <c r="C31">
+        <v>7</v>
+      </c>
+      <c r="D31" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" t="s">
+        <v>87</v>
+      </c>
+      <c r="F31" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>120</v>
+      </c>
+      <c r="B32">
+        <v>2022</v>
+      </c>
+      <c r="C32">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>89</v>
+      </c>
+      <c r="E32" t="s">
+        <v>90</v>
+      </c>
+      <c r="F32" t="s">
+        <v>91</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>120</v>
+      </c>
+      <c r="B33">
+        <v>2022</v>
+      </c>
+      <c r="C33">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>92</v>
+      </c>
+      <c r="E33" t="s">
+        <v>93</v>
+      </c>
+      <c r="F33" t="s">
+        <v>94</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>120</v>
+      </c>
+      <c r="B34">
+        <v>2022</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34" t="s">
+        <v>95</v>
+      </c>
+      <c r="E34" t="s">
+        <v>96</v>
+      </c>
+      <c r="F34" t="s">
+        <v>97</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>120</v>
+      </c>
+      <c r="B35">
+        <v>2022</v>
+      </c>
+      <c r="C35">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>98</v>
+      </c>
+      <c r="E35" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>3</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>120</v>
+      </c>
+      <c r="B36">
+        <v>2022</v>
+      </c>
+      <c r="C36">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>99</v>
+      </c>
+      <c r="E36" t="s">
+        <v>100</v>
+      </c>
+      <c r="F36" t="s">
+        <v>101</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>120</v>
+      </c>
+      <c r="B37">
+        <v>2022</v>
+      </c>
+      <c r="C37">
+        <v>13</v>
+      </c>
+      <c r="D37" t="s">
+        <v>102</v>
+      </c>
+      <c r="E37" t="s">
+        <v>103</v>
+      </c>
+      <c r="F37" t="s">
+        <v>104</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>120</v>
+      </c>
+      <c r="B38">
+        <v>2022</v>
+      </c>
+      <c r="C38">
+        <v>14</v>
+      </c>
+      <c r="D38" t="s">
+        <v>105</v>
+      </c>
+      <c r="E38" t="s">
+        <v>106</v>
+      </c>
+      <c r="F38" t="s">
+        <v>107</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>120</v>
+      </c>
+      <c r="B39">
+        <v>2022</v>
+      </c>
+      <c r="C39">
+        <v>15</v>
+      </c>
+      <c r="D39" t="s">
+        <v>108</v>
+      </c>
+      <c r="E39" t="s">
+        <v>109</v>
+      </c>
+      <c r="F39" t="s">
+        <v>110</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>120</v>
+      </c>
+      <c r="B40">
+        <v>2022</v>
+      </c>
+      <c r="C40">
+        <v>16</v>
+      </c>
+      <c r="D40" t="s">
+        <v>111</v>
+      </c>
+      <c r="E40" t="s">
+        <v>112</v>
+      </c>
+      <c r="F40" t="s">
+        <v>113</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>120</v>
+      </c>
+      <c r="B41">
+        <v>2022</v>
+      </c>
+      <c r="C41">
+        <v>17</v>
+      </c>
+      <c r="D41" t="s">
+        <v>114</v>
+      </c>
+      <c r="E41" t="s">
+        <v>115</v>
+      </c>
+      <c r="F41" t="s">
+        <v>116</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42">
+        <v>2022</v>
+      </c>
+      <c r="C42">
+        <v>18</v>
+      </c>
+      <c r="D42" t="s">
+        <v>117</v>
+      </c>
+      <c r="E42" t="s">
+        <v>118</v>
+      </c>
+      <c r="F42" t="s">
+        <v>119</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>136</v>
+      </c>
+      <c r="B43">
+        <v>2022</v>
+      </c>
+      <c r="C43">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>121</v>
+      </c>
+      <c r="E43" t="s">
+        <v>122</v>
+      </c>
+      <c r="F43" t="s">
+        <v>123</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>136</v>
+      </c>
+      <c r="B44">
+        <v>2022</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>124</v>
+      </c>
+      <c r="E44" t="s">
+        <v>125</v>
+      </c>
+      <c r="F44" t="s">
+        <v>126</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>136</v>
+      </c>
+      <c r="B45">
+        <v>2022</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
+        <v>127</v>
+      </c>
+      <c r="E45" t="s">
+        <v>128</v>
+      </c>
+      <c r="F45" t="s">
+        <v>129</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>136</v>
+      </c>
+      <c r="B46">
+        <v>2022</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s">
+        <v>130</v>
+      </c>
+      <c r="E46" t="s">
+        <v>131</v>
+      </c>
+      <c r="F46" t="s">
+        <v>132</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>136</v>
+      </c>
+      <c r="B47">
+        <v>2022</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47" t="s">
+        <v>133</v>
+      </c>
+      <c r="E47" t="s">
+        <v>134</v>
+      </c>
+      <c r="F47" t="s">
+        <v>135</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>